<commit_message>
changes done on 17th Sep'25
</commit_message>
<xml_diff>
--- a/CVT Workflow/Activity Types.xlsx
+++ b/CVT Workflow/Activity Types.xlsx
@@ -610,4 +610,497 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TCT Non-Client Project Document" ma:contentTypeID="0x010100725E60EF2E824CBB9F9F6219DD094B09A3B1009A1FD45AF037234991198BE85B986831" ma:contentTypeVersion="29" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b20b34f5fe31b8d949247c762e13c773">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e3af3928-72d3-4b8a-b86b-2250b2499d03" xmlns:ns3="ddf28083-347b-4787-8ac1-1645fadd29ee" xmlns:ns4="4aa0ba34-56a9-484a-aec1-7ebf1cb2edb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="814e866c77039ebc108280ef5b820c0c" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="e3af3928-72d3-4b8a-b86b-2250b2499d03"/>
+    <xsd:import namespace="ddf28083-347b-4787-8ac1-1645fadd29ee"/>
+    <xsd:import namespace="4aa0ba34-56a9-484a-aec1-7ebf1cb2edb6"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:TCT_PersonallyIdentifiableInformation" minOccurs="0"/>
+                <xsd:element ref="ns2:TCT_PersonalHealthInformation" minOccurs="0"/>
+                <xsd:element ref="ns2:TCT_ProjectPhase" minOccurs="0"/>
+                <xsd:element ref="ns1:_dlc_Exempt" minOccurs="0"/>
+                <xsd:element ref="ns1:_dlc_ExpireDateSaved" minOccurs="0"/>
+                <xsd:element ref="ns1:_dlc_ExpireDate" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:DateModified" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:Size" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:_Flow_SignoffStatus" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_dlc_Exempt" ma:index="11" nillable="true" ma:displayName="Exempt from Policy" ma:hidden="true" ma:internalName="_dlc_Exempt" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_dlc_ExpireDateSaved" ma:index="12" nillable="true" ma:displayName="Original Expiration Date" ma:hidden="true" ma:internalName="_dlc_ExpireDateSaved" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_dlc_ExpireDate" ma:index="13" nillable="true" ma:displayName="Expiration Date" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="_dlc_ExpireDate" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e3af3928-72d3-4b8a-b86b-2250b2499d03" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TCT_PersonallyIdentifiableInformation" ma:index="8" nillable="true" ma:displayName="PII" ma:default="No" ma:description="Any data about an identifiable individual (such as date of birth or unique ID number)" ma:internalName="TCT_PersonallyIdentifiableInformation">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Yes"/>
+          <xsd:enumeration value="No"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TCT_PersonalHealthInformation" ma:index="9" nillable="true" ma:displayName="PHI(US Only)" ma:default="No" ma:description="For US Projects Only.  Any information from a covered entity about health, coverage, benefits, or payments that can be linked to a specific individual. For details, please see the FAQ section within the Resources site" ma:internalName="TCT_PersonalHealthInformation">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Yes"/>
+          <xsd:enumeration value="No"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TCT_ProjectPhase" ma:index="10" nillable="true" ma:displayName="Project Phase" ma:format="Dropdown" ma:internalName="TCT_ProjectPhase">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Pursue"/>
+          <xsd:enumeration value="Plan, incl. Project Mgmt"/>
+          <xsd:enumeration value="Deliver - Data"/>
+          <xsd:enumeration value="Deliver - Internal Work"/>
+          <xsd:enumeration value="Deliver - Deliverables"/>
+          <xsd:enumeration value="Assess and Close"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="30" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{fbe7246c-a8fb-48fc-9e76-eefdfde83a25}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="4aa0ba34-56a9-484a-aec1-7ebf1cb2edb6">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ddf28083-347b-4787-8ac1-1645fadd29ee" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="14" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="15" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="18" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="19" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="20" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="21" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="22" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="23" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="24" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DateModified" ma:index="25" nillable="true" ma:displayName="Date Modified" ma:format="DateTime" ma:internalName="DateModified">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="29" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5d639306-5220-4f62-8b39-d9a537361609" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Size" ma:index="31" nillable="true" ma:displayName="Size" ma:internalName="Size">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="32" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="33" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_Flow_SignoffStatus" ma:index="34" nillable="true" ma:displayName="Sign-off status" ma:internalName="_x0024_Resources_x003a_core_x002c_Signoff_Status">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4aa0ba34-56a9-484a-aec1-7ebf1cb2edb6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="26" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="27" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>101</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.Policy, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>102</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.Policy, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>103</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.Policy, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>104</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.Policy, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10009</Type>
+    <SequenceNumber>105</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.Policy, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<p:Policy xmlns:p="office.server.policy" id="" local="true">
+  <p:Name>TCT Non-Client Project Document</p:Name>
+  <p:Description/>
+  <p:Statement/>
+  <p:PolicyItems>
+    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration" staticId="0x010100725E60EF2E824CBB9F9F6219DD094B09A3B1|1698352568" UniqueId="fbb21bdb-8079-4a0a-9198-fe05fe82acef">
+      <p:Name>Retention</p:Name>
+      <p:Description>Automatic scheduling of content for processing, and performing a retention action on content that has reached its due date.</p:Description>
+      <p:CustomData>
+        <Schedules nextStageId="3">
+          <Schedule type="Default">
+            <stages>
+              <data stageId="1">
+                <formula id="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration.Formula.BuiltIn">
+                  <number>2</number>
+                  <property>Modified</property>
+                  <propertyId>28cf69c5-fa48-462a-b5cd-27b6f9d2bd5f</propertyId>
+                  <period>years</period>
+                </formula>
+                <action type="action" id="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration.Action.DeletePreviousVersions"/>
+              </data>
+              <data stageId="2">
+                <formula id="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration.Formula.BuiltIn">
+                  <number>10</number>
+                  <property>Modified</property>
+                  <propertyId>28cf69c5-fa48-462a-b5cd-27b6f9d2bd5f</propertyId>
+                  <period>years</period>
+                </formula>
+                <action type="action" id="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration.Action.MoveToRecycleBin"/>
+              </data>
+            </stages>
+          </Schedule>
+        </Schedules>
+      </p:CustomData>
+    </p:PolicyItem>
+  </p:PolicyItems>
+</p:Policy>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="5d639306-5220-4f62-8b39-d9a537361609" ContentTypeId="0x010100725E60EF2E824CBB9F9F6219DD094B09A3" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e3af3928-72d3-4b8a-b86b-2250b2499d03" xsi:nil="true"/>
+    <Size xmlns="ddf28083-347b-4787-8ac1-1645fadd29ee" xsi:nil="true"/>
+    <TCT_PersonalHealthInformation xmlns="e3af3928-72d3-4b8a-b86b-2250b2499d03">No</TCT_PersonalHealthInformation>
+    <TCT_ProjectPhase xmlns="e3af3928-72d3-4b8a-b86b-2250b2499d03" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="ddf28083-347b-4787-8ac1-1645fadd29ee" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ddf28083-347b-4787-8ac1-1645fadd29ee">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TCT_PersonallyIdentifiableInformation xmlns="e3af3928-72d3-4b8a-b86b-2250b2499d03">No</TCT_PersonallyIdentifiableInformation>
+    <DateModified xmlns="ddf28083-347b-4787-8ac1-1645fadd29ee" xsi:nil="true"/>
+    <_dlc_ExpireDateSaved xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_dlc_ExpireDate xmlns="http://schemas.microsoft.com/sharepoint/v3">2027-07-24T13:12:22+00:00</_dlc_ExpireDate>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEF38EB4-E554-44A5-B541-3EE2A4944FC2}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96813B6E-2EB7-44F1-B5AF-634FFD718E9F}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47057A13-7B43-47EC-9E77-10D283477477}"/>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D867130-DB5E-45B6-8D1C-D7899A4AE1E8}"/>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA909AF9-B0B6-41E5-A417-DEAA75C9B249}"/>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{298CF7A3-454C-4604-9E23-BDE9851F35FC}"/>
 </file>
</xml_diff>